<commit_message>
Added logic to categorize pto days and populate with overrides values manually determined.
</commit_message>
<xml_diff>
--- a/python-timesheet-parsing/sample_timesheets/SBAL241011 - partial day.xlsx
+++ b/python-timesheet-parsing/sample_timesheets/SBAL241011 - partial day.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ed7a48ca9db46ee7/Documents/Github/creative-writing-metrics/python-timesheet-parsing/sample_timesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A32260-0D35-4F85-997E-4A1CED2FF08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{A7A32260-0D35-4F85-997E-4A1CED2FF08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{026364C5-BB27-446D-A8AA-C12D664E1EB9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1121,15 +1121,60 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1148,51 +1193,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:O987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1491,20 +1491,20 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="61"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="78"/>
       <c r="M2" s="7"/>
       <c r="N2" s="4"/>
     </row>
@@ -1513,30 +1513,30 @@
       <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="65">
+      <c r="C3" s="90">
         <v>45576</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="64"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="89"/>
       <c r="M3" s="7"/>
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="93" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -1560,7 +1560,7 @@
       <c r="K4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="70" t="s">
+      <c r="L4" s="95" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="11"/>
@@ -1568,9 +1568,9 @@
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1">
       <c r="A5" s="9"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="12">
         <f t="shared" ref="E5:J5" si="0">IF(($C$3=""),"",(F5-1))</f>
         <v>45570</v>
@@ -1599,7 +1599,7 @@
         <f>IF(($C$3=""),"",C3)</f>
         <v>45576</v>
       </c>
-      <c r="L5" s="71"/>
+      <c r="L5" s="96"/>
       <c r="M5" s="11"/>
       <c r="N5" s="4"/>
     </row>
@@ -1644,14 +1644,13 @@
         <v>37</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="16">
+        <v>8</v>
+      </c>
       <c r="H7" s="16">
         <v>4</v>
       </c>
       <c r="I7" s="16"/>
-      <c r="J7" s="16">
-        <v>8</v>
-      </c>
       <c r="K7" s="16"/>
       <c r="L7" s="17">
         <f t="shared" si="1"/>
@@ -1736,18 +1735,18 @@
     </row>
     <row r="11" spans="1:14" ht="16.5" customHeight="1">
       <c r="A11" s="25"/>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="74"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="61"/>
       <c r="L11" s="26">
         <f>SUM(L6:L10)</f>
         <v>20.25</v>
@@ -1757,10 +1756,10 @@
     </row>
     <row r="12" spans="1:14" ht="16.5" customHeight="1">
       <c r="A12" s="25"/>
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="76"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="28"/>
@@ -1793,10 +1792,10 @@
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1">
       <c r="A14" s="19"/>
-      <c r="B14" s="75" t="s">
+      <c r="B14" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="76"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="27"/>
       <c r="E14" s="27"/>
       <c r="F14" s="28"/>
@@ -1897,18 +1896,18 @@
     </row>
     <row r="19" spans="1:15" ht="18" customHeight="1">
       <c r="A19" s="25"/>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="74"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="61"/>
       <c r="L19" s="26">
         <f>SUM(L13:L16)</f>
         <v>0.25</v>
@@ -1918,17 +1917,17 @@
     <row r="20" spans="1:15" ht="18" customHeight="1">
       <c r="A20" s="25"/>
       <c r="B20" s="39"/>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="59"/>
       <c r="E20" s="15">
         <f>SUM(E8:E16)</f>
         <v>0</v>
       </c>
       <c r="F20" s="15">
-        <f>SUM(F8:F16)</f>
-        <v>0</v>
+        <f>SUM(F7:F16)</f>
+        <v>8</v>
       </c>
       <c r="G20" s="17">
         <f t="shared" ref="G20:K20" si="2">SUM(G6:G19)</f>
@@ -1944,7 +1943,7 @@
       </c>
       <c r="J20" s="17">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K20" s="17">
         <f t="shared" si="2"/>
@@ -1958,11 +1957,11 @@
     </row>
     <row r="21" spans="1:15" ht="18" customHeight="1">
       <c r="A21" s="25"/>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="78"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
       <c r="E21" s="15"/>
       <c r="F21" s="40"/>
       <c r="G21" s="41"/>
@@ -1996,66 +1995,66 @@
     </row>
     <row r="23" spans="1:15" ht="18" customHeight="1">
       <c r="A23" s="5"/>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="88" t="s">
+      <c r="C23" s="61"/>
+      <c r="D23" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="73"/>
-      <c r="F23" s="89"/>
-      <c r="G23" s="93" t="s">
+      <c r="E23" s="71"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="86">
+      <c r="H23" s="77"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="68">
         <f>L20</f>
         <v>21.5</v>
       </c>
-      <c r="L23" s="87"/>
+      <c r="L23" s="69"/>
       <c r="M23" s="43"/>
     </row>
     <row r="24" spans="1:15" ht="18" customHeight="1">
       <c r="A24" s="5"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="93" t="s">
+      <c r="B24" s="62"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="94">
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="79">
         <f>IF(32-K23&gt;0,32-K23, 0)</f>
         <v>10.5</v>
       </c>
-      <c r="L24" s="95"/>
+      <c r="L24" s="80"/>
       <c r="M24" s="43"/>
     </row>
     <row r="25" spans="1:15" ht="18" customHeight="1">
       <c r="A25" s="5"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="84" t="s">
+      <c r="B25" s="63"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="96">
+      <c r="H25" s="66"/>
+      <c r="I25" s="66"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="81">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="L25" s="87"/>
+      <c r="L25" s="69"/>
       <c r="M25" s="43"/>
     </row>
     <row r="26" spans="1:15" ht="18" customHeight="1">
@@ -2067,20 +2066,20 @@
         <f>C3</f>
         <v>45576</v>
       </c>
-      <c r="D26" s="82"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="92"/>
-      <c r="G26" s="84" t="s">
+      <c r="D26" s="63"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="86">
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="68">
         <f>K23+K24</f>
         <v>32</v>
       </c>
-      <c r="L26" s="87"/>
+      <c r="L26" s="69"/>
       <c r="M26" s="43"/>
     </row>
     <row r="27" spans="1:15" ht="18" customHeight="1">
@@ -18421,6 +18420,18 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B19:K19"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B23:C25"/>
     <mergeCell ref="G26:J26"/>
@@ -18432,18 +18443,6 @@
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="G25:J25"/>
     <mergeCell ref="K25:L25"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B19:K19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:L3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="L4:L5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0" header="0" footer="0"/>

</xml_diff>